<commit_message>
Development of renmas2 begin.
</commit_message>
<xml_diff>
--- a/AlphaRenmasTasks.xlsx
+++ b/AlphaRenmasTasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Preparation for Spectral Rendering</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Next after obj</t>
   </si>
 </sst>
 </file>
@@ -507,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +549,9 @@
       <c r="F7" s="3">
         <v>40856</v>
       </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
@@ -555,7 +564,7 @@
         <v>40703</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -644,6 +653,9 @@
       </c>
       <c r="F16" t="s">
         <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>